<commit_message>
Pre and Post processing functions for Benchmarking and added values in excel
</commit_message>
<xml_diff>
--- a/Benchmarking data.xlsx
+++ b/Benchmarking data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSA\Project\INFO-6205-Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F473CC82-DF81-4761-A095-CFC9B3453C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44DE278-93E4-48FD-BD60-3502A5E647C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Sorting Method</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Husky Sort</t>
+  </si>
+  <si>
+    <t>PreProcess</t>
+  </si>
+  <si>
+    <t>MEAN:- 4056</t>
+  </si>
+  <si>
+    <t>PostProcess</t>
+  </si>
+  <si>
+    <t>Mean:- 945</t>
   </si>
 </sst>
 </file>
@@ -381,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:L194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,11 +1013,11 @@
       <c r="C42">
         <v>100</v>
       </c>
-      <c r="D42">
-        <v>689</v>
+      <c r="D42" s="1">
+        <v>20401</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1016,10 +1028,10 @@
         <v>100</v>
       </c>
       <c r="D43" s="1">
-        <v>1873</v>
+        <v>47311</v>
       </c>
       <c r="E43">
-        <v>18</v>
+        <v>473</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1030,10 +1042,10 @@
         <v>100</v>
       </c>
       <c r="D44" s="1">
-        <v>4894</v>
+        <v>94582</v>
       </c>
       <c r="E44">
-        <v>48</v>
+        <v>945</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1044,10 +1056,10 @@
         <v>100</v>
       </c>
       <c r="D45" s="1">
-        <v>13565</v>
-      </c>
-      <c r="E45">
-        <v>135</v>
+        <v>197454</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1974</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,10 +1070,10 @@
         <v>100</v>
       </c>
       <c r="D46" s="1">
-        <v>13620</v>
-      </c>
-      <c r="E46">
-        <v>136</v>
+        <v>413292</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4132</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1072,10 +1084,10 @@
         <v>200</v>
       </c>
       <c r="D47" s="1">
-        <v>1426</v>
+        <v>40528</v>
       </c>
       <c r="E47">
-        <v>7</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1086,10 +1098,10 @@
         <v>200</v>
       </c>
       <c r="D48" s="1">
-        <v>3207</v>
+        <v>93716</v>
       </c>
       <c r="E48">
-        <v>16</v>
+        <v>468</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,10 +1112,10 @@
         <v>200</v>
       </c>
       <c r="D49" s="1">
-        <v>6296</v>
+        <v>174761</v>
       </c>
       <c r="E49">
-        <v>31</v>
+        <v>873</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,10 +1126,10 @@
         <v>200</v>
       </c>
       <c r="D50" s="1">
-        <v>11934</v>
-      </c>
-      <c r="E50">
-        <v>59</v>
+        <v>371344</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1856</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,10 +1140,10 @@
         <v>200</v>
       </c>
       <c r="D51" s="1">
-        <v>21039</v>
-      </c>
-      <c r="E51">
-        <v>105</v>
+        <v>857471</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4287</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,10 +1154,10 @@
         <v>400</v>
       </c>
       <c r="D52" s="1">
-        <v>2100</v>
+        <v>82013</v>
       </c>
       <c r="E52">
-        <v>5</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1156,10 +1168,10 @@
         <v>400</v>
       </c>
       <c r="D53" s="1">
-        <v>5403</v>
+        <v>189479</v>
       </c>
       <c r="E53">
-        <v>13</v>
+        <v>473</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,10 +1182,10 @@
         <v>400</v>
       </c>
       <c r="D54" s="1">
-        <v>11670</v>
+        <v>359207</v>
       </c>
       <c r="E54">
-        <v>29</v>
+        <v>898</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1184,10 +1196,10 @@
         <v>400</v>
       </c>
       <c r="D55" s="1">
-        <v>25152</v>
-      </c>
-      <c r="E55">
-        <v>62</v>
+        <v>769075</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1922</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1198,10 +1210,10 @@
         <v>400</v>
       </c>
       <c r="D56" s="1">
-        <v>70032</v>
-      </c>
-      <c r="E56">
-        <v>175</v>
+        <v>1589627</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3974</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1212,10 +1224,10 @@
         <v>800</v>
       </c>
       <c r="D57" s="1">
-        <v>5187</v>
+        <v>166442</v>
       </c>
       <c r="E57">
-        <v>6</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1226,10 +1238,10 @@
         <v>800</v>
       </c>
       <c r="D58" s="1">
-        <v>11788</v>
+        <v>368943</v>
       </c>
       <c r="E58">
-        <v>14</v>
+        <v>461</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,10 +1252,10 @@
         <v>800</v>
       </c>
       <c r="D59" s="1">
-        <v>20477</v>
+        <v>739329</v>
       </c>
       <c r="E59">
-        <v>25</v>
+        <v>924</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1254,10 +1266,10 @@
         <v>800</v>
       </c>
       <c r="D60" s="3">
-        <v>65775</v>
-      </c>
-      <c r="E60" s="2">
-        <v>82</v>
+        <v>1493178</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1866</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1268,10 +1280,10 @@
         <v>800</v>
       </c>
       <c r="D61" s="1">
-        <v>117346</v>
-      </c>
-      <c r="E61">
-        <v>146</v>
+        <v>3398146</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4247</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1671,6 +1683,820 @@
       </c>
       <c r="E89" s="1">
         <v>26674</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>4516</v>
+      </c>
+      <c r="C95">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>4090</v>
+      </c>
+      <c r="C96">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>3664</v>
+      </c>
+      <c r="C97">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>3628</v>
+      </c>
+      <c r="C98">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>3827</v>
+      </c>
+      <c r="C99">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>4105</v>
+      </c>
+      <c r="C100">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>3634</v>
+      </c>
+      <c r="C101">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>3739</v>
+      </c>
+      <c r="C102">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>3872</v>
+      </c>
+      <c r="C103">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>4143</v>
+      </c>
+      <c r="C104">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>3781</v>
+      </c>
+      <c r="C105">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>3674</v>
+      </c>
+      <c r="C106">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>3630</v>
+      </c>
+      <c r="C107">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>3963</v>
+      </c>
+      <c r="C108">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>3824</v>
+      </c>
+      <c r="C109">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>3612</v>
+      </c>
+      <c r="C110">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>3961</v>
+      </c>
+      <c r="C111">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>3704</v>
+      </c>
+      <c r="C112">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>3857</v>
+      </c>
+      <c r="C113">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>3795</v>
+      </c>
+      <c r="C114">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>4101</v>
+      </c>
+      <c r="C115">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>3582</v>
+      </c>
+      <c r="C116">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>3674</v>
+      </c>
+      <c r="C117">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>3661</v>
+      </c>
+      <c r="C118">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>4094</v>
+      </c>
+      <c r="C119">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>3726</v>
+      </c>
+      <c r="C120">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>4470</v>
+      </c>
+      <c r="C121">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>4326</v>
+      </c>
+      <c r="C122">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>4558</v>
+      </c>
+      <c r="C123">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>4536</v>
+      </c>
+      <c r="C124">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>5023</v>
+      </c>
+      <c r="C125">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>4752</v>
+      </c>
+      <c r="C126">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>4580</v>
+      </c>
+      <c r="C127">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>4949</v>
+      </c>
+      <c r="C128">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>4387</v>
+      </c>
+      <c r="C129">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>4064</v>
+      </c>
+      <c r="C130">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>4473</v>
+      </c>
+      <c r="C131">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>5211</v>
+      </c>
+      <c r="C132">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>4472</v>
+      </c>
+      <c r="C133">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>4316</v>
+      </c>
+      <c r="C134">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>4177</v>
+      </c>
+      <c r="C135">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>4201</v>
+      </c>
+      <c r="C136">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>4279</v>
+      </c>
+      <c r="C137">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>4380</v>
+      </c>
+      <c r="C138">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>4101</v>
+      </c>
+      <c r="C139">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>4139</v>
+      </c>
+      <c r="C140">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>4331</v>
+      </c>
+      <c r="C141">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>4216</v>
+      </c>
+      <c r="C142">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>4018</v>
+      </c>
+      <c r="C143">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>3859</v>
+      </c>
+      <c r="C144">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>4429</v>
+      </c>
+      <c r="C145">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>3851</v>
+      </c>
+      <c r="C146">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>4652</v>
+      </c>
+      <c r="C147">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>4338</v>
+      </c>
+      <c r="C148">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>4103</v>
+      </c>
+      <c r="C149">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>4298</v>
+      </c>
+      <c r="C150">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>4441</v>
+      </c>
+      <c r="C151">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>5276</v>
+      </c>
+      <c r="C152">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>4630</v>
+      </c>
+      <c r="C153">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>5057</v>
+      </c>
+      <c r="C154">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>5100</v>
+      </c>
+      <c r="C155">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>4257</v>
+      </c>
+      <c r="C156">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>4188</v>
+      </c>
+      <c r="C157">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>4347</v>
+      </c>
+      <c r="C158">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>3926</v>
+      </c>
+      <c r="C159">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>3809</v>
+      </c>
+      <c r="C160">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>3957</v>
+      </c>
+      <c r="C161">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>3616</v>
+      </c>
+      <c r="C162">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>3883</v>
+      </c>
+      <c r="C163">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>3725</v>
+      </c>
+      <c r="C164">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>3616</v>
+      </c>
+      <c r="C165">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>3668</v>
+      </c>
+      <c r="C166">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>3733</v>
+      </c>
+      <c r="C167">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>3776</v>
+      </c>
+      <c r="C168">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>3819</v>
+      </c>
+      <c r="C169">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>3804</v>
+      </c>
+      <c r="C170">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>4047</v>
+      </c>
+      <c r="C171">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>4079</v>
+      </c>
+      <c r="C172">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>3728</v>
+      </c>
+      <c r="C173">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>3863</v>
+      </c>
+      <c r="C174">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>3848</v>
+      </c>
+      <c r="C175">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>4106</v>
+      </c>
+      <c r="C176">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>3918</v>
+      </c>
+      <c r="C177">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>3846</v>
+      </c>
+      <c r="C178">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>3850</v>
+      </c>
+      <c r="C179">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>3802</v>
+      </c>
+      <c r="C180">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>3892</v>
+      </c>
+      <c r="C181">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>3730</v>
+      </c>
+      <c r="C182">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>3616</v>
+      </c>
+      <c r="C183">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>3889</v>
+      </c>
+      <c r="C184">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>3693</v>
+      </c>
+      <c r="C185">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>3933</v>
+      </c>
+      <c r="C186">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>3890</v>
+      </c>
+      <c r="C187">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>3645</v>
+      </c>
+      <c r="C188">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>3650</v>
+      </c>
+      <c r="C189">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>3646</v>
+      </c>
+      <c r="C190">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>3694</v>
+      </c>
+      <c r="C191">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>3697</v>
+      </c>
+      <c r="C192">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>3822</v>
+      </c>
+      <c r="C193">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>3838</v>
+      </c>
+      <c r="C194">
+        <v>961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>